<commit_message>
Add names to the top row
</commit_message>
<xml_diff>
--- a/top_three_contributors.xlsx
+++ b/top_three_contributors.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,6 +421,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Yu Qiao</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Luc Van Gool</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Lei Zhang</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -439,6 +456,13 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Total</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Insert information to the file
</commit_message>
<xml_diff>
--- a/top_three_contributors.xlsx
+++ b/top_three_contributors.xlsx
@@ -444,6 +444,15 @@
           <t>2022</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -451,6 +460,15 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -458,11 +476,35 @@
           <t>2024</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>26</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Total</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Yu Qiao</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Luc Van Gool</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Lei Zhang</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the total row
</commit_message>
<xml_diff>
--- a/top_three_contributors.xlsx
+++ b/top_three_contributors.xlsx
@@ -492,20 +492,14 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Yu Qiao</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Luc Van Gool</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Lei Zhang</t>
-        </is>
+      <c r="B5" t="n">
+        <v>55</v>
+      </c>
+      <c r="C5" t="n">
+        <v>54</v>
+      </c>
+      <c r="D5" t="n">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>